<commit_message>
TCTC_04 with extent reports
</commit_message>
<xml_diff>
--- a/src/main/java/NopCommerceDemo/Reports/Credential.xlsx
+++ b/src/main/java/NopCommerceDemo/Reports/Credential.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\honey\IdeaProjects\NopCommerceDemo\src\main\java\NopCommerceDemo\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8851993A-8BA6-4A72-8193-762425BDAEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A515AEA-D11C-4AD3-95D6-A36E44BB9C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3684" yWindow="5724" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3684" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>UserName</t>
   </si>
@@ -58,6 +59,36 @@
   </si>
   <si>
     <t>Random123</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>FaxNumber</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Random #103 Delhi India</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -388,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -443,4 +474,74 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8E8D4F-E31F-404D-98CE-100A68A34951}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>123456</v>
+      </c>
+      <c r="F2">
+        <v>9876543210</v>
+      </c>
+      <c r="G2">
+        <v>55555555</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TCTC_02 with extent reports
</commit_message>
<xml_diff>
--- a/src/main/java/NopCommerceDemo/Reports/Credential.xlsx
+++ b/src/main/java/NopCommerceDemo/Reports/Credential.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\honey\IdeaProjects\NopCommerceDemo\src\main\java\NopCommerceDemo\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8851993A-8BA6-4A72-8193-762425BDAEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A515AEA-D11C-4AD3-95D6-A36E44BB9C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3684" yWindow="5724" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3684" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>UserName</t>
   </si>
@@ -58,6 +59,36 @@
   </si>
   <si>
     <t>Random123</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>FaxNumber</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Random #103 Delhi India</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -388,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -443,4 +474,74 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8E8D4F-E31F-404D-98CE-100A68A34951}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>123456</v>
+      </c>
+      <c r="F2">
+        <v>9876543210</v>
+      </c>
+      <c r="G2">
+        <v>55555555</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TCTC_01 with extent reports
</commit_message>
<xml_diff>
--- a/src/main/java/NopCommerceDemo/Reports/Credential.xlsx
+++ b/src/main/java/NopCommerceDemo/Reports/Credential.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\honey\IdeaProjects\NopCommerceDemo\src\main\java\NopCommerceDemo\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8851993A-8BA6-4A72-8193-762425BDAEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B27BFAD-5CE7-468B-A885-D1D71E1C7A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3684" yWindow="5724" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3684" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>UserName</t>
   </si>
@@ -58,6 +59,30 @@
   </si>
   <si>
     <t>Random123</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>FaxNumber</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Random #103 Delhi India</t>
   </si>
 </sst>
 </file>
@@ -388,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -443,4 +468,68 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8E8D4F-E31F-404D-98CE-100A68A34951}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>123456</v>
+      </c>
+      <c r="E2">
+        <v>9876543210</v>
+      </c>
+      <c r="F2">
+        <v>55555555</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>